<commit_message>
update table formats csv/xls
</commit_message>
<xml_diff>
--- a/SMHI_project_handwritten_weather_journals-master/table_formats.xlsx
+++ b/SMHI_project_handwritten_weather_journals-master/table_formats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valte\Desktop\Python\SMHI-computer-vision\SMHI_project_handwritten_weather_journals-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29AC8E0D-3338-470D-84A9-D6BCE66D7F9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E45D2034-C0B0-4CEE-86CF-F0D1931A8FA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -429,8 +429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A128" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G140" sqref="G140:I143"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J28" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>